<commit_message>
Updated the Excel document with all of our names
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECEUWO\Teaching\Fall2017\SE3352A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\Year3SE\SE3352A\Assignment\Loop-Solutions-Inc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,21 +42,6 @@
   </si>
   <si>
     <t>P: Primary   S: Support</t>
-  </si>
-  <si>
-    <t>Team Member 2</t>
-  </si>
-  <si>
-    <t>Team Member 3</t>
-  </si>
-  <si>
-    <t>Team Member 4</t>
-  </si>
-  <si>
-    <t>Team Member 5</t>
-  </si>
-  <si>
-    <t>Team Member 6</t>
   </si>
   <si>
     <t xml:space="preserve">Team Name: </t>
@@ -91,20 +76,22 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Team Member 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Replace it by the correct team member name</t>
-    </r>
+    <t>Andrew Black</t>
+  </si>
+  <si>
+    <t>Samuel Mallabone</t>
+  </si>
+  <si>
+    <t>Jak Terpak</t>
+  </si>
+  <si>
+    <t>Craig Cook</t>
+  </si>
+  <si>
+    <t>Robert Northmore</t>
+  </si>
+  <si>
+    <t>Stephanie Pereira</t>
   </si>
 </sst>
 </file>
@@ -139,9 +126,9 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
@@ -205,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +210,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,30 +531,30 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="47.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.89453125" style="1"/>
+    <col min="2" max="2" width="47.89453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.41796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,39 +564,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="1:8" ht="30.9" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="6">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -619,12 +609,12 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -639,7 +629,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
@@ -649,7 +639,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="6"/>
@@ -659,7 +649,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="6"/>
@@ -669,7 +659,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
@@ -679,7 +669,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="6"/>
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
@@ -689,7 +679,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="6"/>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
@@ -699,7 +689,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
@@ -709,7 +699,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="6"/>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
@@ -719,10 +709,10 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>

</xml_diff>

<commit_message>
Completed a few Sections, Testing  branch push
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\Year3SE\SE3352A\Assignment\Loop-Solutions-Inc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\School\Year3\SE3352\Group Work\Assignment1\Loop-Solutions-Inc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -38,67 +38,104 @@
     <t>P</t>
   </si>
   <si>
+    <t>P: Primary   S: Support</t>
+  </si>
+  <si>
+    <t>Andrew Black</t>
+  </si>
+  <si>
+    <t>Samuel Mallabone</t>
+  </si>
+  <si>
+    <t>Jak Terpak</t>
+  </si>
+  <si>
+    <t>Craig Cook</t>
+  </si>
+  <si>
+    <t>Robert Northmore</t>
+  </si>
+  <si>
+    <t>Stephanie Pereira</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS - Section 1.2 </t>
+  </si>
+  <si>
+    <t>SRS - Section 1.3</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.4</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.5</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.2</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.2</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.3</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.4</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.5</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.6</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.7</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.8</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.9</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.11</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.12</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.13</t>
+  </si>
+  <si>
+    <t>Team Name: Loop Solutions Inc.</t>
+  </si>
+  <si>
+    <t>Project Name: Self-Start Physiotherapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>P: Primary   S: Support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team Name: </t>
-  </si>
-  <si>
-    <t>Project Name:</t>
-  </si>
-  <si>
-    <t>&lt;Add rows as necessary&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Enter task name, section number, or sib section number as it appears in the SRS template breakdown here&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Example)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SRS - Section 3.2</t>
-    </r>
-  </si>
-  <si>
-    <t>Andrew Black</t>
-  </si>
-  <si>
-    <t>Samuel Mallabone</t>
-  </si>
-  <si>
-    <t>Jak Terpak</t>
-  </si>
-  <si>
-    <t>Craig Cook</t>
-  </si>
-  <si>
-    <t>Robert Northmore</t>
-  </si>
-  <si>
-    <t>Stephanie Pereira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,25 +157,43 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -192,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -202,18 +257,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,198 +591,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="1"/>
-    <col min="2" max="2" width="47.89453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.41796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="47.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.89453125" style="1"/>
+    <col min="7" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="5" spans="1:8" ht="30.9" thickBot="1" x14ac:dyDescent="0.6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="C8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="6">
+      <c r="C11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="5">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5">
+        <v>3</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Draft to be editted
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -44,38 +44,6 @@
     <t>P: Primary   S: Support</t>
   </si>
   <si>
-    <t xml:space="preserve">Team Name: </t>
-  </si>
-  <si>
-    <t>Project Name:</t>
-  </si>
-  <si>
-    <t>&lt;Add rows as necessary&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Enter task name, section number, or sib section number as it appears in the SRS template breakdown here&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Example)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SRS - Section 3.2</t>
-    </r>
-  </si>
-  <si>
     <t>Andrew Black</t>
   </si>
   <si>
@@ -92,13 +60,79 @@
   </si>
   <si>
     <t>Stephanie Pereira</t>
+  </si>
+  <si>
+    <t>Team Name: Loop Solutions Inc.</t>
+  </si>
+  <si>
+    <t>Project Name: Self-Start Physiotherapy</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS - Section 1.2 </t>
+  </si>
+  <si>
+    <t>SRS - Section 1.3</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.4</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.5</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.2</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.2</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.3</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.4</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.5</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.6</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.7</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.8</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.9</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.11</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.12</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,25 +154,43 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -192,7 +244,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -202,18 +259,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -547,179 +609,418 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="30.9" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="5" spans="1:8" ht="30.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="8">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="6">
+      <c r="B11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="A13" s="8">
+        <v>3</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="8">
+        <v>3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="8">
+        <v>3</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="8">
+        <v>3</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="8">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="8">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="8">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A21" s="8">
+        <v>3</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="8">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A23" s="8">
+        <v>3</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="8">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="8">
+        <v>3</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
changes to some patients, updated the responsibility matrix
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\School\Year3\SE3352\Group Work\Assignment2\Loop-Solutions-Inc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\Year3SE\Semester 2\SE3350B\Loop-Solutions-Inc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -138,6 +138,54 @@
   </si>
   <si>
     <t>Work Done as a team</t>
+  </si>
+  <si>
+    <t>Semester 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Semester 2</t>
+  </si>
+  <si>
+    <t>Created 3 Routes</t>
+  </si>
+  <si>
+    <t>Revised Schemas</t>
+  </si>
+  <si>
+    <t>Revision explanation</t>
+  </si>
+  <si>
+    <t>Created 5 tables</t>
+  </si>
+  <si>
+    <t>Added 2 routes</t>
+  </si>
+  <si>
+    <t>Configured .gitignore</t>
+  </si>
+  <si>
+    <t>Edited SDS document</t>
+  </si>
+  <si>
+    <t>Wrote technical decision SDS section</t>
+  </si>
+  <si>
+    <t>Created 4 tables</t>
+  </si>
+  <si>
+    <t>Revised all routes</t>
+  </si>
+  <si>
+    <t>Manage Dynamic Forms Questions</t>
+  </si>
+  <si>
+    <t>Manage Rehabilitation Plans</t>
+  </si>
+  <si>
+    <t>Manage Exercises</t>
+  </si>
+  <si>
+    <t>Manage Patient Profiles</t>
   </si>
 </sst>
 </file>
@@ -256,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -282,15 +330,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,26 +656,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="47.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.89453125" style="1"/>
+    <col min="2" max="2" width="47.89453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.41796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -632,18 +684,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="22.2" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="1:14" ht="30.9" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -669,28 +721,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -701,44 +749,34 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="14" t="s">
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>3</v>
@@ -758,48 +796,56 @@
       <c r="H9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="5">
         <v>1.2</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>17</v>
+      <c r="B12" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>3</v>
@@ -812,12 +858,12 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>18</v>
+        <v>1.2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>3</v>
@@ -830,44 +876,46 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="5">
         <v>1.3</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="B14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="5">
         <v>1.3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="5">
         <v>1.3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -878,12 +926,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="5">
         <v>1.3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -894,28 +942,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="5">
         <v>1.3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H18" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="5">
         <v>1.3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -926,12 +974,12 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="5">
         <v>1.3</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -942,12 +990,12 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5">
         <v>1.3</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -958,46 +1006,44 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5">
         <v>1.3</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="F22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="5">
         <v>1.3</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24" s="5">
         <v>1.3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>3</v>
@@ -1010,123 +1056,133 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A26" s="5">
         <v>2.1</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="5">
+      <c r="C26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A27" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5">
+      <c r="C27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A28" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="5">
+      <c r="C28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A29" s="5">
         <v>2.4</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="5"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="5"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -1134,75 +1190,495 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4"/>
+    <row r="31" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A31" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5"/>
-      <c r="B32" s="4"/>
+    <row r="32" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A32" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="5"/>
-      <c r="B33" s="4"/>
+    <row r="33" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A33" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="5"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
+    <row r="34" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A34" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="5"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
+    <row r="35" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A35" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="5"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
+    <row r="36" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A36" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="5"/>
-      <c r="B37" s="4"/>
+    <row r="37" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A37" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A38" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A41" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A42" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A43" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A44" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A45" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A46" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A47" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A48" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A49" s="5"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A51" s="5"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A52" s="5"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A53" s="5"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A55" s="5"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A56" s="5"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A57" s="5"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A59" s="5"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A60" s="5"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A62" s="5"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A63" s="5"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A65" s="5"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A66" s="5"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A67" s="5"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A68" s="5"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
final changes made before submitting
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="70">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -207,6 +207,33 @@
   </si>
   <si>
     <t>Created Template For Scheduler</t>
+  </si>
+  <si>
+    <t>Complete Assessment Test</t>
+  </si>
+  <si>
+    <t>Added Encryption Service for Delicate Information</t>
+  </si>
+  <si>
+    <t>Manage Test Assessments</t>
+  </si>
+  <si>
+    <t>Manage Findings and Outcomes</t>
+  </si>
+  <si>
+    <t>Assign Patient Plan</t>
+  </si>
+  <si>
+    <t>Complete Exercises</t>
+  </si>
+  <si>
+    <t>Finished the Scheduler</t>
+  </si>
+  <si>
+    <t>Landing Pages - Home, About, etc..</t>
+  </si>
+  <si>
+    <t>Landing Pages - Physiotherapist, Admin</t>
   </si>
 </sst>
 </file>
@@ -680,9 +707,9 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -1618,9 +1645,15 @@
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A56" s="5"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="5"/>
+      <c r="A56" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -1628,9 +1661,15 @@
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A57" s="5"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="5"/>
+      <c r="A57" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -1638,74 +1677,116 @@
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A58" s="5"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A59" s="5"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A60" s="5"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A61" s="5"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A62" s="5"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="G62" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="5"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="F63" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="5"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
+      <c r="H64" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="65" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A65" s="5"/>

</xml_diff>